<commit_message>
Thay đoi file excel mot chut
</commit_message>
<xml_diff>
--- a/Huan/FB-Cleaned/BasicML.xlsx
+++ b/Huan/FB-Cleaned/BasicML.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Minh Hoang\source\repos\Teamb_Scraping_data\Huan\FB-Cleaned\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D774FE0-1F4D-4CC8-9000-B6A58444D60D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F606D093-CE6B-4B23-BADF-6CE9E68932FD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="150" yWindow="5580" windowWidth="20490" windowHeight="5640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -451,9 +451,6 @@
     <t>Email</t>
   </si>
   <si>
-    <t>Phone Number</t>
-  </si>
-  <si>
     <t xml:space="preserve">Salary </t>
   </si>
   <si>
@@ -515,6 +512,9 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>SDT</t>
   </si>
 </sst>
 </file>
@@ -950,17 +950,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H2412"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D28" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="18.28515625" customWidth="1"/>
-    <col min="3" max="3" width="107.140625" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="40.28515625" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" customWidth="1"/>
+    <col min="3" max="3" width="31" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="13" customWidth="1"/>
+    <col min="6" max="6" width="25.7109375" customWidth="1"/>
     <col min="7" max="7" width="19.28515625" customWidth="1"/>
     <col min="8" max="8" width="10.140625" customWidth="1"/>
   </cols>
@@ -973,13 +973,13 @@
         <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>142</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>143</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>2</v>
@@ -999,7 +999,7 @@
         <v>34</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G2" t="s">
         <v>70</v>
@@ -1019,13 +1019,13 @@
         <v>35</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E3" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="F3" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="G3" t="s">
         <v>71</v>
@@ -1045,7 +1045,7 @@
         <v>36</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G4" t="s">
         <v>73</v>
@@ -1065,10 +1065,10 @@
         <v>37</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="E5" t="s">
-        <v>145</v>
+        <v>163</v>
+      </c>
+      <c r="F5" t="s">
+        <v>144</v>
       </c>
       <c r="G5" t="s">
         <v>72</v>
@@ -1088,7 +1088,7 @@
         <v>38</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G6" t="s">
         <v>74</v>
@@ -1108,7 +1108,7 @@
         <v>39</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G7" t="s">
         <v>75</v>
@@ -1128,7 +1128,7 @@
         <v>40</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G8" t="s">
         <v>76</v>
@@ -1148,7 +1148,7 @@
         <v>41</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G9" t="s">
         <v>77</v>
@@ -1168,7 +1168,7 @@
         <v>42</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G10" t="s">
         <v>78</v>
@@ -1188,7 +1188,7 @@
         <v>43</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G11" t="s">
         <v>79</v>
@@ -1208,7 +1208,7 @@
         <v>44</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G12" t="s">
         <v>80</v>
@@ -1228,7 +1228,7 @@
         <v>45</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G13" t="s">
         <v>81</v>
@@ -1248,7 +1248,7 @@
         <v>46</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G14" t="s">
         <v>82</v>
@@ -1268,7 +1268,7 @@
         <v>47</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G15" t="s">
         <v>83</v>
@@ -1288,7 +1288,7 @@
         <v>48</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G16" t="s">
         <v>84</v>
@@ -1308,7 +1308,7 @@
         <v>49</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G17" t="s">
         <v>85</v>
@@ -1328,7 +1328,7 @@
         <v>50</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G18" t="s">
         <v>86</v>
@@ -1348,7 +1348,7 @@
         <v>51</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G19" t="s">
         <v>87</v>
@@ -1368,7 +1368,7 @@
         <v>52</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G20" t="s">
         <v>88</v>
@@ -1388,7 +1388,7 @@
         <v>53</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G21" t="s">
         <v>89</v>
@@ -1408,7 +1408,7 @@
         <v>54</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G22" t="s">
         <v>90</v>
@@ -1428,7 +1428,7 @@
         <v>55</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G23" t="s">
         <v>91</v>
@@ -1448,10 +1448,10 @@
         <v>56</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="E24" t="s">
-        <v>146</v>
+        <v>163</v>
+      </c>
+      <c r="F24" t="s">
+        <v>145</v>
       </c>
       <c r="G24" t="s">
         <v>92</v>
@@ -1471,7 +1471,7 @@
         <v>57</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G25" t="s">
         <v>93</v>
@@ -1491,10 +1491,10 @@
         <v>58</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="E26" t="s">
-        <v>149</v>
+        <v>155</v>
+      </c>
+      <c r="F26" t="s">
+        <v>148</v>
       </c>
       <c r="G26" t="s">
         <v>94</v>
@@ -1514,7 +1514,7 @@
         <v>59</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G27" t="s">
         <v>95</v>
@@ -1534,10 +1534,10 @@
         <v>60</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="E28" t="s">
-        <v>147</v>
+        <v>163</v>
+      </c>
+      <c r="F28" t="s">
+        <v>146</v>
       </c>
       <c r="G28" t="s">
         <v>96</v>
@@ -1557,7 +1557,7 @@
         <v>61</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G29" t="s">
         <v>97</v>
@@ -1577,10 +1577,10 @@
         <v>62</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="E30" t="s">
-        <v>150</v>
+        <v>154</v>
+      </c>
+      <c r="F30" t="s">
+        <v>149</v>
       </c>
       <c r="G30" t="s">
         <v>98</v>
@@ -1600,7 +1600,7 @@
         <v>63</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G31" t="s">
         <v>99</v>
@@ -1620,7 +1620,7 @@
         <v>64</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G32" t="s">
         <v>100</v>
@@ -1640,10 +1640,10 @@
         <v>65</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="E33" t="s">
-        <v>152</v>
+        <v>163</v>
+      </c>
+      <c r="F33" t="s">
+        <v>151</v>
       </c>
       <c r="G33" t="s">
         <v>101</v>
@@ -1663,10 +1663,10 @@
         <v>66</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="E34" t="s">
-        <v>151</v>
+        <v>163</v>
+      </c>
+      <c r="F34" t="s">
+        <v>150</v>
       </c>
       <c r="G34" t="s">
         <v>102</v>
@@ -1686,7 +1686,7 @@
         <v>67</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G35" t="s">
         <v>103</v>
@@ -1706,7 +1706,7 @@
         <v>68</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G36" t="s">
         <v>104</v>
@@ -1726,7 +1726,7 @@
         <v>69</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G37" t="s">
         <v>105</v>

</xml_diff>